<commit_message>
spreadsheet handling, home page styling
</commit_message>
<xml_diff>
--- a/temp.xlsx
+++ b/temp.xlsx
@@ -4,9 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
-    <sheet sheetId="1" name="Instructions" state="visible" r:id="rId4"/>
-    <sheet sheetId="2" name="Metadata" state="visible" r:id="rId5"/>
-    <sheet sheetId="3" name=" Data" state="visible" r:id="rId6"/>
+    <sheet sheetId="1" name="undefined Data" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027" fullCalcOnLoad="1"/>
 </workbook>
@@ -15,7 +13,17 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
-    <t xml:space="preserve"> Audit</t>
+    <r>
+      <rPr>
+        <b/>
+        <color theme="1"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+        <sz val="18"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>undefined Audit</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -40,7 +48,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <bgColor rgb="cfe2f3"/>
+        <fgColor rgb="cfe2f3"/>
       </patternFill>
     </fill>
   </fills>
@@ -56,8 +64,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" indent="2"/>
+      <protection hidden="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyProtection="1">
       <protection hidden="1"/>
     </xf>
@@ -400,22 +412,6 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A1"/>
-  <sheetFormatPr customHeight="1"/>
-  <sheetData/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A1"/>
-  <sheetFormatPr customHeight="1"/>
-  <sheetData/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L4"/>
   <sheetFormatPr customHeight="1"/>
   <sheetData>
@@ -427,13 +423,13 @@
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
@@ -441,13 +437,13 @@
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
@@ -455,13 +451,13 @@
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B4"/>

</xml_diff>